<commit_message>
Cleaning + Adding README
</commit_message>
<xml_diff>
--- a/data/HF_quantification_data.xlsx
+++ b/data/HF_quantification_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\R\Bnip3\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\mar\Dev\Projects\R\Bnip3_McGill_AD\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D60115A6-92FC-4ED1-A82D-E52E35AC3F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E844383-B891-485C-A301-44F274F90C03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1875" yWindow="2115" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,9 +41,6 @@
     <t>Background</t>
   </si>
   <si>
-    <t>Bnip3-level</t>
-  </si>
-  <si>
     <t>Age</t>
   </si>
   <si>
@@ -56,10 +53,13 @@
     <t>AD</t>
   </si>
   <si>
-    <t>X</t>
+    <t>WT</t>
   </si>
   <si>
-    <t>WT</t>
+    <t>OD</t>
+  </si>
+  <si>
+    <t>OD Corrected</t>
   </si>
 </sst>
 </file>
@@ -392,27 +392,27 @@
   <dimension ref="A1:F187"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="9.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.3828125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.84375" customWidth="1"/>
+    <col min="6" max="6" width="15.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>6</v>
@@ -421,15 +421,15 @@
         <v>0</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>26702</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -445,12 +445,12 @@
         <v>0.16500000000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>26702</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -466,12 +466,12 @@
         <v>0.16160000000000008</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>26702</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -487,12 +487,12 @@
         <v>0.17969999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>26702</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -508,12 +508,12 @@
         <v>0.17210000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>26702</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -529,12 +529,12 @@
         <v>0.16469999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>26702</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -550,12 +550,12 @@
         <v>0.33779999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>26702</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8">
         <v>3</v>
@@ -571,12 +571,12 @@
         <v>0.23340000000000005</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>26701</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -592,12 +592,12 @@
         <v>0.12390000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>26701</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10">
         <v>3</v>
@@ -613,12 +613,12 @@
         <v>4.2200000000000015E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>26701</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11">
         <v>3</v>
@@ -634,12 +634,12 @@
         <v>0.13960000000000006</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>26701</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12">
         <v>3</v>
@@ -655,12 +655,12 @@
         <v>8.6099999999999954E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>26701</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13">
         <v>3</v>
@@ -676,12 +676,12 @@
         <v>9.9500000000000033E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>26701</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14">
         <v>3</v>
@@ -697,12 +697,12 @@
         <v>0.10760000000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>26701</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C15">
         <v>3</v>
@@ -718,12 +718,12 @@
         <v>0.18840000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>26703</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C16">
         <v>3</v>
@@ -739,12 +739,12 @@
         <v>0.25050000000000006</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>26703</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17">
         <v>3</v>
@@ -760,12 +760,12 @@
         <v>0.21869999999999989</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>26703</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C18">
         <v>3</v>
@@ -781,12 +781,12 @@
         <v>0.33199999999999985</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>26703</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C19">
         <v>3</v>
@@ -802,12 +802,12 @@
         <v>0.30829999999999991</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>26703</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C20">
         <v>3</v>
@@ -823,12 +823,12 @@
         <v>0.35960000000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>26703</v>
       </c>
       <c r="B21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C21">
         <v>3</v>
@@ -844,12 +844,12 @@
         <v>0.28600000000000003</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>26703</v>
       </c>
       <c r="B22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C22">
         <v>3</v>
@@ -865,12 +865,12 @@
         <v>0.24609999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>26703</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C23">
         <v>3</v>
@@ -886,12 +886,12 @@
         <v>0.2410000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>26705</v>
       </c>
       <c r="B24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C24">
         <v>3</v>
@@ -907,12 +907,12 @@
         <v>0.35149999999999992</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>26705</v>
       </c>
       <c r="B25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C25">
         <v>3</v>
@@ -928,12 +928,12 @@
         <v>0.32679999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>26705</v>
       </c>
       <c r="B26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C26">
         <v>3</v>
@@ -949,12 +949,12 @@
         <v>0.34539999999999993</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>26705</v>
       </c>
       <c r="B27" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C27">
         <v>3</v>
@@ -970,12 +970,12 @@
         <v>0.36959999999999993</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>26705</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C28">
         <v>3</v>
@@ -991,12 +991,12 @@
         <v>0.38959999999999995</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>26705</v>
       </c>
       <c r="B29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C29">
         <v>3</v>
@@ -1012,12 +1012,12 @@
         <v>0.37369999999999992</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>26705</v>
       </c>
       <c r="B30" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C30">
         <v>3</v>
@@ -1033,12 +1033,12 @@
         <v>0.36370000000000013</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>15727</v>
       </c>
       <c r="B31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C31">
         <v>12</v>
@@ -1054,12 +1054,12 @@
         <v>9.8100000000000076E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>15727</v>
       </c>
       <c r="B32" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C32">
         <v>12</v>
@@ -1075,12 +1075,12 @@
         <v>0.10370000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>15727</v>
       </c>
       <c r="B33" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C33">
         <v>12</v>
@@ -1096,12 +1096,12 @@
         <v>0.10519999999999996</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A34">
         <v>15727</v>
       </c>
       <c r="B34" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C34">
         <v>12</v>
@@ -1117,12 +1117,12 @@
         <v>8.6199999999999943E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>15727</v>
       </c>
       <c r="B35" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C35">
         <v>12</v>
@@ -1138,12 +1138,12 @@
         <v>6.8900000000000072E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A36">
         <v>15727</v>
       </c>
       <c r="B36" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C36">
         <v>12</v>
@@ -1159,12 +1159,12 @@
         <v>6.9500000000000006E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>15727</v>
       </c>
       <c r="B37" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C37">
         <v>12</v>
@@ -1180,12 +1180,12 @@
         <v>4.1800000000000059E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A38">
         <v>15727</v>
       </c>
       <c r="B38" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C38">
         <v>12</v>
@@ -1201,12 +1201,12 @@
         <v>5.9699999999999975E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A39">
         <v>15866</v>
       </c>
       <c r="B39" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C39">
         <v>12</v>
@@ -1222,12 +1222,12 @@
         <v>8.7799999999999989E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A40">
         <v>15866</v>
       </c>
       <c r="B40" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C40">
         <v>12</v>
@@ -1243,12 +1243,12 @@
         <v>6.4899999999999958E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A41">
         <v>15866</v>
       </c>
       <c r="B41" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C41">
         <v>12</v>
@@ -1264,12 +1264,12 @@
         <v>7.3699999999999988E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A42">
         <v>15866</v>
       </c>
       <c r="B42" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C42">
         <v>12</v>
@@ -1285,12 +1285,12 @@
         <v>7.6200000000000045E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A43">
         <v>15866</v>
       </c>
       <c r="B43" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C43">
         <v>12</v>
@@ -1306,12 +1306,12 @@
         <v>7.7099999999999946E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A44">
         <v>15866</v>
       </c>
       <c r="B44" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C44">
         <v>12</v>
@@ -1327,12 +1327,12 @@
         <v>8.7100000000000066E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A45">
         <v>15866</v>
       </c>
       <c r="B45" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C45">
         <v>12</v>
@@ -1348,12 +1348,12 @@
         <v>5.4200000000000026E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A46">
         <v>15866</v>
       </c>
       <c r="B46" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C46">
         <v>12</v>
@@ -1369,12 +1369,12 @@
         <v>7.6500000000000012E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A47">
         <v>15868</v>
       </c>
       <c r="B47" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C47">
         <v>12</v>
@@ -1390,12 +1390,12 @@
         <v>5.7599999999999985E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A48">
         <v>15868</v>
       </c>
       <c r="B48" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C48">
         <v>12</v>
@@ -1411,12 +1411,12 @@
         <v>4.9299999999999899E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A49">
         <v>15868</v>
       </c>
       <c r="B49" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C49">
         <v>12</v>
@@ -1432,12 +1432,12 @@
         <v>3.8600000000000079E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A50">
         <v>15868</v>
       </c>
       <c r="B50" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C50">
         <v>12</v>
@@ -1453,12 +1453,12 @@
         <v>4.720000000000002E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A51">
         <v>15868</v>
       </c>
       <c r="B51" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C51">
         <v>12</v>
@@ -1474,12 +1474,12 @@
         <v>7.9399999999999915E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A52">
         <v>15868</v>
       </c>
       <c r="B52" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C52">
         <v>12</v>
@@ -1495,12 +1495,12 @@
         <v>6.4200000000000035E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A53">
         <v>15868</v>
       </c>
       <c r="B53" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C53">
         <v>12</v>
@@ -1516,12 +1516,12 @@
         <v>3.8799999999999946E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A54">
         <v>15868</v>
       </c>
       <c r="B54" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C54">
         <v>12</v>
@@ -1537,12 +1537,12 @@
         <v>7.4500000000000066E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A55">
         <v>15873</v>
       </c>
       <c r="B55" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C55">
         <v>12</v>
@@ -1558,12 +1558,12 @@
         <v>7.6200000000000045E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A56">
         <v>15873</v>
       </c>
       <c r="B56" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C56">
         <v>12</v>
@@ -1579,12 +1579,12 @@
         <v>6.3200000000000034E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A57">
         <v>15873</v>
       </c>
       <c r="B57" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C57">
         <v>12</v>
@@ -1600,12 +1600,12 @@
         <v>8.0199999999999938E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A58">
         <v>15873</v>
       </c>
       <c r="B58" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C58">
         <v>12</v>
@@ -1621,12 +1621,12 @@
         <v>4.6000000000000041E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A59">
         <v>15873</v>
       </c>
       <c r="B59" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C59">
         <v>12</v>
@@ -1642,12 +1642,12 @@
         <v>7.2899999999999965E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A60">
         <v>15873</v>
       </c>
       <c r="B60" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C60">
         <v>12</v>
@@ -1663,12 +1663,12 @@
         <v>5.4199999999999915E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A61">
         <v>15873</v>
       </c>
       <c r="B61" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C61">
         <v>12</v>
@@ -1684,12 +1684,12 @@
         <v>7.779999999999998E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A62">
         <v>15873</v>
       </c>
       <c r="B62" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C62">
         <v>12</v>
@@ -1705,12 +1705,12 @@
         <v>4.049999999999998E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A63">
         <v>20291</v>
       </c>
       <c r="B63" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C63">
         <v>18</v>
@@ -1726,12 +1726,12 @@
         <v>5.2899999999999947E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A64">
         <v>20291</v>
       </c>
       <c r="B64" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C64">
         <v>18</v>
@@ -1747,12 +1747,12 @@
         <v>8.1100000000000005E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A65">
         <v>20291</v>
       </c>
       <c r="B65" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C65">
         <v>18</v>
@@ -1768,12 +1768,12 @@
         <v>6.9199999999999984E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A66">
         <v>20291</v>
       </c>
       <c r="B66" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C66">
         <v>18</v>
@@ -1789,12 +1789,12 @@
         <v>3.0299999999999938E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A67">
         <v>20291</v>
       </c>
       <c r="B67" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C67">
         <v>18</v>
@@ -1810,12 +1810,12 @@
         <v>5.5300000000000016E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A68">
         <v>20291</v>
       </c>
       <c r="B68" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C68">
         <v>18</v>
@@ -1831,12 +1831,12 @@
         <v>3.4799999999999998E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A69">
         <v>20291</v>
       </c>
       <c r="B69" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C69">
         <v>18</v>
@@ -1852,12 +1852,12 @@
         <v>4.2999999999999983E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A70">
         <v>20291</v>
       </c>
       <c r="B70" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C70">
         <v>18</v>
@@ -1873,12 +1873,12 @@
         <v>5.2699999999999969E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A71">
         <v>23520</v>
       </c>
       <c r="B71" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C71">
         <v>18</v>
@@ -1894,12 +1894,12 @@
         <v>9.1899999999999982E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A72">
         <v>23520</v>
       </c>
       <c r="B72" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C72">
         <v>18</v>
@@ -1915,12 +1915,12 @@
         <v>0.10639999999999994</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A73">
         <v>23520</v>
       </c>
       <c r="B73" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C73">
         <v>18</v>
@@ -1936,12 +1936,12 @@
         <v>5.2100000000000035E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A74">
         <v>23520</v>
       </c>
       <c r="B74" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C74">
         <v>18</v>
@@ -1957,12 +1957,12 @@
         <v>0.10370000000000001</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A75">
         <v>23520</v>
       </c>
       <c r="B75" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C75">
         <v>18</v>
@@ -1978,12 +1978,12 @@
         <v>0.10589999999999999</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A76">
         <v>23520</v>
       </c>
       <c r="B76" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C76">
         <v>18</v>
@@ -1999,12 +1999,12 @@
         <v>0.12350000000000005</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A77">
         <v>23520</v>
       </c>
       <c r="B77" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C77">
         <v>18</v>
@@ -2020,12 +2020,12 @@
         <v>0.14300000000000002</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A78">
         <v>23520</v>
       </c>
       <c r="B78" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C78">
         <v>18</v>
@@ -2041,12 +2041,12 @@
         <v>0.14300000000000002</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A79">
         <v>23747</v>
       </c>
       <c r="B79" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C79">
         <v>18</v>
@@ -2062,12 +2062,12 @@
         <v>0.12739999999999996</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A80">
         <v>23747</v>
       </c>
       <c r="B80" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C80">
         <v>18</v>
@@ -2083,12 +2083,12 @@
         <v>0.17220000000000002</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A81">
         <v>23747</v>
       </c>
       <c r="B81" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C81">
         <v>18</v>
@@ -2104,12 +2104,12 @@
         <v>0.16080000000000005</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A82">
         <v>23747</v>
       </c>
       <c r="B82" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C82">
         <v>18</v>
@@ -2125,12 +2125,12 @@
         <v>0.16479999999999995</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A83">
         <v>23747</v>
       </c>
       <c r="B83" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C83">
         <v>18</v>
@@ -2146,12 +2146,12 @@
         <v>0.19699999999999995</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A84">
         <v>23747</v>
       </c>
       <c r="B84" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C84">
         <v>18</v>
@@ -2167,12 +2167,12 @@
         <v>0.10089999999999999</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A85">
         <v>23747</v>
       </c>
       <c r="B85" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C85">
         <v>18</v>
@@ -2188,12 +2188,12 @@
         <v>0.12949999999999995</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A86">
         <v>23747</v>
       </c>
       <c r="B86" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C86">
         <v>18</v>
@@ -2209,12 +2209,12 @@
         <v>0.10819999999999996</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A87" s="1">
         <v>26141</v>
       </c>
       <c r="B87" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C87">
         <v>18</v>
@@ -2230,12 +2230,12 @@
         <v>8.6399999999999921E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A88" s="1">
         <v>26141</v>
       </c>
       <c r="B88" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C88">
         <v>18</v>
@@ -2251,12 +2251,12 @@
         <v>8.2999999999999963E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A89" s="1">
         <v>26141</v>
       </c>
       <c r="B89" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C89">
         <v>18</v>
@@ -2272,12 +2272,12 @@
         <v>7.1699999999999986E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A90" s="1">
         <v>26141</v>
       </c>
       <c r="B90" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C90">
         <v>18</v>
@@ -2293,12 +2293,12 @@
         <v>0.11110000000000009</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A91" s="1">
         <v>26141</v>
       </c>
       <c r="B91" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C91">
         <v>18</v>
@@ -2314,12 +2314,12 @@
         <v>7.46E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A92" s="1">
         <v>26141</v>
       </c>
       <c r="B92" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C92">
         <v>18</v>
@@ -2335,12 +2335,12 @@
         <v>4.7800000000000065E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A93" s="1">
         <v>26141</v>
       </c>
       <c r="B93" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C93">
         <v>18</v>
@@ -2356,12 +2356,12 @@
         <v>6.0099999999999931E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A94" s="1">
         <v>26141</v>
       </c>
       <c r="B94" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C94">
         <v>18</v>
@@ -2377,12 +2377,12 @@
         <v>7.4400000000000022E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A95">
         <v>17679</v>
       </c>
       <c r="B95" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C95">
         <v>3</v>
@@ -2397,12 +2397,12 @@
         <v>7.1500000000000008E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A96">
         <v>17679</v>
       </c>
       <c r="B96" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C96">
         <v>3</v>
@@ -2417,12 +2417,12 @@
         <v>9.2400000000000038E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A97">
         <v>17679</v>
       </c>
       <c r="B97" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C97">
         <v>3</v>
@@ -2437,12 +2437,12 @@
         <v>8.8399999999999923E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A98">
         <v>17679</v>
       </c>
       <c r="B98" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C98">
         <v>3</v>
@@ -2457,12 +2457,12 @@
         <v>7.7300000000000035E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A99">
         <v>17679</v>
       </c>
       <c r="B99" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C99">
         <v>3</v>
@@ -2477,12 +2477,12 @@
         <v>7.7100000000000057E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A100">
         <v>17679</v>
       </c>
       <c r="B100" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C100">
         <v>3</v>
@@ -2497,12 +2497,12 @@
         <v>8.0799999999999983E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A101">
         <v>17679</v>
       </c>
       <c r="B101" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C101">
         <v>3</v>
@@ -2517,12 +2517,12 @@
         <v>9.0400000000000036E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A102">
         <v>17679</v>
       </c>
       <c r="B102" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C102">
         <v>3</v>
@@ -2537,12 +2537,12 @@
         <v>5.7299999999999907E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A103">
         <v>17709</v>
       </c>
       <c r="B103" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C103">
         <v>3</v>
@@ -2557,12 +2557,12 @@
         <v>4.599999999999993E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A104">
         <v>17709</v>
       </c>
       <c r="B104" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C104">
         <v>3</v>
@@ -2577,12 +2577,12 @@
         <v>8.7399999999999922E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A105">
         <v>17709</v>
       </c>
       <c r="B105" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C105">
         <v>3</v>
@@ -2597,12 +2597,12 @@
         <v>8.6099999999999954E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A106">
         <v>17709</v>
       </c>
       <c r="B106" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C106">
         <v>3</v>
@@ -2617,12 +2617,12 @@
         <v>9.8500000000000032E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A107">
         <v>17709</v>
       </c>
       <c r="B107" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C107">
         <v>3</v>
@@ -2637,12 +2637,12 @@
         <v>7.9199999999999937E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A108">
         <v>17709</v>
       </c>
       <c r="B108" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C108">
         <v>3</v>
@@ -2657,12 +2657,12 @@
         <v>0.11239999999999994</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A109">
         <v>17709</v>
       </c>
       <c r="B109" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C109">
         <v>3</v>
@@ -2677,12 +2677,12 @@
         <v>8.3799999999999986E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A110">
         <v>17709</v>
       </c>
       <c r="B110" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C110">
         <v>3</v>
@@ -2697,12 +2697,12 @@
         <v>9.5199999999999951E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A111">
         <v>26759</v>
       </c>
       <c r="B111" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C111">
         <v>3</v>
@@ -2717,12 +2717,12 @@
         <v>0.15920000000000001</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A112">
         <v>26759</v>
       </c>
       <c r="B112" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C112">
         <v>3</v>
@@ -2737,12 +2737,12 @@
         <v>0.29899999999999993</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A113">
         <v>26759</v>
       </c>
       <c r="B113" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C113">
         <v>3</v>
@@ -2757,12 +2757,12 @@
         <v>0.18470000000000009</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A114">
         <v>26759</v>
       </c>
       <c r="B114" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C114">
         <v>3</v>
@@ -2777,12 +2777,12 @@
         <v>0.35820000000000007</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A115">
         <v>26759</v>
       </c>
       <c r="B115" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C115">
         <v>3</v>
@@ -2797,12 +2797,12 @@
         <v>0.32409999999999994</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A116">
         <v>26759</v>
       </c>
       <c r="B116" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C116">
         <v>3</v>
@@ -2817,12 +2817,12 @@
         <v>0.20689999999999997</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A117">
         <v>26759</v>
       </c>
       <c r="B117" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C117">
         <v>3</v>
@@ -2837,12 +2837,12 @@
         <v>0.16999999999999993</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A118">
         <v>26759</v>
       </c>
       <c r="B118" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C118">
         <v>3</v>
@@ -2857,12 +2857,12 @@
         <v>0.24609999999999999</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A119">
         <v>26760</v>
       </c>
       <c r="B119" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C119">
         <v>3</v>
@@ -2877,12 +2877,12 @@
         <v>0.1643</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A120">
         <v>26760</v>
       </c>
       <c r="B120" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C120">
         <v>3</v>
@@ -2897,12 +2897,12 @@
         <v>0.12840000000000007</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A121">
         <v>26760</v>
       </c>
       <c r="B121" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C121">
         <v>3</v>
@@ -2917,12 +2917,12 @@
         <v>0.13590000000000002</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A122">
         <v>26760</v>
       </c>
       <c r="B122" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C122">
         <v>3</v>
@@ -2937,12 +2937,12 @@
         <v>0.19489999999999996</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A123">
         <v>26760</v>
       </c>
       <c r="B123" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C123">
         <v>3</v>
@@ -2957,12 +2957,12 @@
         <v>0.14949999999999997</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A124">
         <v>26760</v>
       </c>
       <c r="B124" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C124">
         <v>3</v>
@@ -2977,12 +2977,12 @@
         <v>5.0799999999999956E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A125">
         <v>26760</v>
       </c>
       <c r="B125" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C125">
         <v>3</v>
@@ -2997,12 +2997,12 @@
         <v>0.13829999999999998</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A126">
         <v>26343</v>
       </c>
       <c r="B126" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C126">
         <v>12</v>
@@ -3017,12 +3017,12 @@
         <v>5.3099999999999925E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A127">
         <v>26343</v>
       </c>
       <c r="B127" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C127">
         <v>12</v>
@@ -3037,12 +3037,12 @@
         <v>6.3000000000000056E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A128">
         <v>26343</v>
       </c>
       <c r="B128" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C128">
         <v>12</v>
@@ -3057,12 +3057,12 @@
         <v>1.1700000000000044E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A129">
         <v>26343</v>
       </c>
       <c r="B129" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C129">
         <v>12</v>
@@ -3077,12 +3077,12 @@
         <v>0.14379999999999993</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A130">
         <v>26343</v>
       </c>
       <c r="B130" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C130">
         <v>12</v>
@@ -3097,12 +3097,12 @@
         <v>0.10310000000000008</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A131">
         <v>26343</v>
       </c>
       <c r="B131" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C131">
         <v>12</v>
@@ -3117,12 +3117,12 @@
         <v>9.0900000000000092E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A132">
         <v>26343</v>
       </c>
       <c r="B132" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C132">
         <v>12</v>
@@ -3137,12 +3137,12 @@
         <v>9.6300000000000052E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A133">
         <v>26343</v>
       </c>
       <c r="B133" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C133">
         <v>12</v>
@@ -3157,12 +3157,12 @@
         <v>8.5899999999999976E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A134">
         <v>26344</v>
       </c>
       <c r="B134" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C134">
         <v>12</v>
@@ -3177,12 +3177,12 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A135">
         <v>26344</v>
       </c>
       <c r="B135" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C135">
         <v>12</v>
@@ -3197,12 +3197,12 @@
         <v>0.15880000000000005</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A136">
         <v>26344</v>
       </c>
       <c r="B136" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C136">
         <v>12</v>
@@ -3217,12 +3217,12 @@
         <v>2.1199999999999997E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A137">
         <v>26344</v>
       </c>
       <c r="B137" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C137">
         <v>12</v>
@@ -3237,12 +3237,12 @@
         <v>3.9799999999999947E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A138">
         <v>26344</v>
       </c>
       <c r="B138" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C138">
         <v>12</v>
@@ -3257,12 +3257,12 @@
         <v>0.14139999999999997</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A139">
         <v>26344</v>
       </c>
       <c r="B139" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C139">
         <v>12</v>
@@ -3277,12 +3277,12 @@
         <v>0.3892000000000001</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A140">
         <v>26344</v>
       </c>
       <c r="B140" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C140">
         <v>12</v>
@@ -3297,12 +3297,12 @@
         <v>0.12490000000000001</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A141">
         <v>26344</v>
       </c>
       <c r="B141" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C141">
         <v>12</v>
@@ -3317,12 +3317,12 @@
         <v>6.9900000000000073E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A142">
         <v>26345</v>
       </c>
       <c r="B142" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C142">
         <v>12</v>
@@ -3337,12 +3337,12 @@
         <v>0.11830000000000007</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A143">
         <v>26345</v>
       </c>
       <c r="B143" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C143">
         <v>12</v>
@@ -3357,12 +3357,12 @@
         <v>7.020000000000004E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A144">
         <v>26345</v>
       </c>
       <c r="B144" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C144">
         <v>12</v>
@@ -3377,12 +3377,12 @@
         <v>0.12039999999999995</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A145">
         <v>26345</v>
       </c>
       <c r="B145" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C145">
         <v>12</v>
@@ -3397,12 +3397,12 @@
         <v>8.6000000000000076E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A146">
         <v>26345</v>
       </c>
       <c r="B146" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C146">
         <v>12</v>
@@ -3417,12 +3417,12 @@
         <v>0.1431</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A147">
         <v>26345</v>
       </c>
       <c r="B147" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C147">
         <v>12</v>
@@ -3437,12 +3437,12 @@
         <v>4.5200000000000018E-2</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A148">
         <v>26345</v>
       </c>
       <c r="B148" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C148">
         <v>12</v>
@@ -3457,12 +3457,12 @@
         <v>8.2499999999999907E-2</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A149">
         <v>26345</v>
       </c>
       <c r="B149" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C149">
         <v>12</v>
@@ -3477,12 +3477,12 @@
         <v>8.0899999999999972E-2</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A150">
         <v>26346</v>
       </c>
       <c r="B150" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C150">
         <v>12</v>
@@ -3497,12 +3497,12 @@
         <v>4.1200000000000014E-2</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A151">
         <v>26346</v>
       </c>
       <c r="B151" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C151">
         <v>12</v>
@@ -3517,12 +3517,12 @@
         <v>6.9200000000000039E-2</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A152">
         <v>26346</v>
       </c>
       <c r="B152" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C152">
         <v>12</v>
@@ -3537,12 +3537,12 @@
         <v>4.9600000000000088E-2</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A153">
         <v>26346</v>
       </c>
       <c r="B153" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C153">
         <v>12</v>
@@ -3557,12 +3557,12 @@
         <v>6.9500000000000006E-2</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A154">
         <v>26346</v>
       </c>
       <c r="B154" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C154">
         <v>12</v>
@@ -3577,12 +3577,12 @@
         <v>6.7599999999999993E-2</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A155">
         <v>26346</v>
       </c>
       <c r="B155" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C155">
         <v>12</v>
@@ -3597,12 +3597,12 @@
         <v>5.2400000000000002E-2</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A156">
         <v>26346</v>
       </c>
       <c r="B156" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C156">
         <v>12</v>
@@ -3617,12 +3617,12 @@
         <v>5.8800000000000074E-2</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A157">
         <v>26346</v>
       </c>
       <c r="B157" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C157">
         <v>12</v>
@@ -3637,12 +3637,12 @@
         <v>9.2499999999999916E-2</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A158">
         <v>26141</v>
       </c>
       <c r="B158" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C158">
         <v>18</v>
@@ -3657,12 +3657,12 @@
         <v>8.4300000000000042E-2</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A159">
         <v>26141</v>
       </c>
       <c r="B159" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C159">
         <v>18</v>
@@ -3677,12 +3677,12 @@
         <v>5.7500000000000051E-2</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A160">
         <v>26141</v>
       </c>
       <c r="B160" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C160">
         <v>18</v>
@@ -3697,12 +3697,12 @@
         <v>5.3300000000000014E-2</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A161">
         <v>26141</v>
       </c>
       <c r="B161" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C161">
         <v>18</v>
@@ -3717,12 +3717,12 @@
         <v>2.1099999999999952E-2</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A162">
         <v>26141</v>
       </c>
       <c r="B162" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C162">
         <v>18</v>
@@ -3737,12 +3737,12 @@
         <v>3.9800000000000002E-2</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A163">
         <v>26141</v>
       </c>
       <c r="B163" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C163">
         <v>18</v>
@@ -3757,12 +3757,12 @@
         <v>3.3999999999999975E-2</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A164">
         <v>26141</v>
       </c>
       <c r="B164" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C164">
         <v>18</v>
@@ -3777,12 +3777,12 @@
         <v>3.5600000000000021E-2</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A165">
         <v>26141</v>
       </c>
       <c r="B165" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C165">
         <v>18</v>
@@ -3797,12 +3797,12 @@
         <v>1.1599999999999999E-2</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A166">
         <v>26142</v>
       </c>
       <c r="B166" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C166">
         <v>18</v>
@@ -3817,12 +3817,12 @@
         <v>2.1499999999999964E-2</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A167">
         <v>26142</v>
       </c>
       <c r="B167" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C167">
         <v>18</v>
@@ -3837,12 +3837,12 @@
         <v>4.1799999999999948E-2</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A168">
         <v>26142</v>
       </c>
       <c r="B168" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C168">
         <v>18</v>
@@ -3857,12 +3857,12 @@
         <v>2.1600000000000064E-2</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A169">
         <v>26142</v>
       </c>
       <c r="B169" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C169">
         <v>18</v>
@@ -3877,12 +3877,12 @@
         <v>4.500000000000004E-2</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A170">
         <v>26142</v>
       </c>
       <c r="B170" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C170">
         <v>18</v>
@@ -3897,12 +3897,12 @@
         <v>1.7299999999999982E-2</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A171">
         <v>26142</v>
       </c>
       <c r="B171" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C171">
         <v>18</v>
@@ -3917,12 +3917,12 @@
         <v>2.3899999999999921E-2</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A172">
         <v>26142</v>
       </c>
       <c r="B172" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C172">
         <v>18</v>
@@ -3937,12 +3937,12 @@
         <v>1.9199999999999995E-2</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A173">
         <v>26143</v>
       </c>
       <c r="B173" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C173">
         <v>18</v>
@@ -3957,12 +3957,12 @@
         <v>6.3799999999999968E-2</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A174">
         <v>26143</v>
       </c>
       <c r="B174" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C174">
         <v>18</v>
@@ -3977,12 +3977,12 @@
         <v>4.5199999999999962E-2</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A175">
         <v>26143</v>
       </c>
       <c r="B175" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C175">
         <v>18</v>
@@ -3997,12 +3997,12 @@
         <v>2.1100000000000008E-2</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A176">
         <v>26143</v>
       </c>
       <c r="B176" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C176">
         <v>18</v>
@@ -4017,12 +4017,12 @@
         <v>4.7599999999999976E-2</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A177">
         <v>26143</v>
       </c>
       <c r="B177" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C177">
         <v>18</v>
@@ -4037,12 +4037,12 @@
         <v>4.2700000000000016E-2</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A178">
         <v>26143</v>
       </c>
       <c r="B178" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C178">
         <v>18</v>
@@ -4057,12 +4057,12 @@
         <v>3.8599999999999968E-2</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A179">
         <v>26143</v>
       </c>
       <c r="B179" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C179">
         <v>18</v>
@@ -4077,12 +4077,12 @@
         <v>4.2200000000000015E-2</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A180">
         <v>26144</v>
       </c>
       <c r="B180" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C180">
         <v>18</v>
@@ -4097,12 +4097,12 @@
         <v>1.6199999999999992E-2</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A181">
         <v>26144</v>
       </c>
       <c r="B181" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C181">
         <v>18</v>
@@ -4117,12 +4117,12 @@
         <v>2.3499999999999965E-2</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A182">
         <v>26144</v>
       </c>
       <c r="B182" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C182">
         <v>18</v>
@@ -4137,12 +4137,12 @@
         <v>3.2000000000000028E-2</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A183">
         <v>26144</v>
       </c>
       <c r="B183" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C183">
         <v>18</v>
@@ -4157,12 +4157,12 @@
         <v>5.8699999999999974E-2</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A184">
         <v>26144</v>
       </c>
       <c r="B184" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C184">
         <v>18</v>
@@ -4177,12 +4177,12 @@
         <v>8.1300000000000039E-2</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A185">
         <v>26144</v>
       </c>
       <c r="B185" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C185">
         <v>18</v>
@@ -4197,12 +4197,12 @@
         <v>3.1500000000000083E-2</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A186">
         <v>26144</v>
       </c>
       <c r="B186" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C186">
         <v>18</v>
@@ -4217,12 +4217,12 @@
         <v>4.2899999999999938E-2</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A187">
         <v>26144</v>
       </c>
       <c r="B187" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C187">
         <v>18</v>

</xml_diff>